<commit_message>
Update 2022-09-20 #5 - Update excel files.
</commit_message>
<xml_diff>
--- a/Excels/ข้อมูลผู้ใช้สิทธิปี 2562 350 เขต.xlsx
+++ b/Excels/ข้อมูลผู้ใช้สิทธิปี 2562 350 เขต.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="ข้อมูลผู้ใช้สิทธิ 350 เขต" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ข้อมูลผู้ใช้สิทธิ 350 เขต'!$A$1:$I$351</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
@@ -771,9 +774,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I351"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -783,7 +789,7 @@
     <col min="4" max="4" width="35.88671875" customWidth="1"/>
     <col min="5" max="5" width="27.21875" customWidth="1"/>
     <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.21875" customWidth="1"/>
     <col min="8" max="8" width="28.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
   </cols>
@@ -817,7 +823,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="20.399999999999999">
+    <row r="2" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
@@ -846,7 +852,7 @@
         <v>2.0151872586646009</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="20.399999999999999">
+    <row r="3" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
@@ -875,7 +881,7 @@
         <v>2.2124574316159507</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="20.399999999999999">
+    <row r="4" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A4" s="8" t="s">
         <v>7</v>
       </c>
@@ -904,7 +910,7 @@
         <v>2.1637497662446235</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="20.399999999999999">
+    <row r="5" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A5" s="8" t="s">
         <v>7</v>
       </c>
@@ -933,7 +939,7 @@
         <v>2.0559844449302207</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="20.399999999999999">
+    <row r="6" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
@@ -962,7 +968,7 @@
         <v>1.7468741720722338</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="20.399999999999999">
+    <row r="7" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A7" s="8" t="s">
         <v>7</v>
       </c>
@@ -991,7 +997,7 @@
         <v>2.0473430755437243</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="20.399999999999999">
+    <row r="8" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A8" s="8" t="s">
         <v>7</v>
       </c>
@@ -1020,7 +1026,7 @@
         <v>2.1069067216685622</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="20.399999999999999">
+    <row r="9" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
@@ -1049,7 +1055,7 @@
         <v>1.7228364637449491</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="20.399999999999999">
+    <row r="10" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A10" s="8" t="s">
         <v>7</v>
       </c>
@@ -1078,7 +1084,7 @@
         <v>1.9443791617704662</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="20.399999999999999">
+    <row r="11" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A11" s="8" t="s">
         <v>7</v>
       </c>
@@ -1107,7 +1113,7 @@
         <v>2.0326248146317352</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="20.399999999999999">
+    <row r="12" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A12" s="8" t="s">
         <v>7</v>
       </c>
@@ -1136,7 +1142,7 @@
         <v>1.4761396915680598</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="20.399999999999999">
+    <row r="13" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A13" s="8" t="s">
         <v>7</v>
       </c>
@@ -1165,7 +1171,7 @@
         <v>1.927457058209032</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="20.399999999999999">
+    <row r="14" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A14" s="8" t="s">
         <v>7</v>
       </c>
@@ -1194,7 +1200,7 @@
         <v>1.7443669576995589</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="20.399999999999999">
+    <row r="15" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A15" s="8" t="s">
         <v>7</v>
       </c>
@@ -1223,7 +1229,7 @@
         <v>1.6784057722040886</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="20.399999999999999">
+    <row r="16" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A16" s="8" t="s">
         <v>7</v>
       </c>
@@ -1252,7 +1258,7 @@
         <v>1.5866806602423433</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="20.399999999999999">
+    <row r="17" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A17" s="8" t="s">
         <v>7</v>
       </c>
@@ -1281,7 +1287,7 @@
         <v>1.7424646048230024</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="20.399999999999999">
+    <row r="18" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A18" s="8" t="s">
         <v>7</v>
       </c>
@@ -1310,7 +1316,7 @@
         <v>1.6978068282255248</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="20.399999999999999">
+    <row r="19" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A19" s="8" t="s">
         <v>7</v>
       </c>
@@ -1339,7 +1345,7 @@
         <v>1.6585483676180508</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="20.399999999999999">
+    <row r="20" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A20" s="8" t="s">
         <v>7</v>
       </c>
@@ -1368,7 +1374,7 @@
         <v>1.7314534695663755</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="20.399999999999999">
+    <row r="21" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A21" s="8" t="s">
         <v>7</v>
       </c>
@@ -1397,7 +1403,7 @@
         <v>2.0270551508844954</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="20.399999999999999">
+    <row r="22" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A22" s="8" t="s">
         <v>7</v>
       </c>
@@ -1426,7 +1432,7 @@
         <v>2.1435371729158454</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="20.399999999999999">
+    <row r="23" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A23" s="8" t="s">
         <v>7</v>
       </c>
@@ -1455,7 +1461,7 @@
         <v>2.2282266054219582</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="20.399999999999999">
+    <row r="24" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A24" s="8" t="s">
         <v>7</v>
       </c>
@@ -1484,7 +1490,7 @@
         <v>1.8610541024409415</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="20.399999999999999">
+    <row r="25" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A25" s="8" t="s">
         <v>7</v>
       </c>
@@ -1513,7 +1519,7 @@
         <v>2.1830787969643026</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="20.399999999999999">
+    <row r="26" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A26" s="8" t="s">
         <v>7</v>
       </c>
@@ -1542,7 +1548,7 @@
         <v>1.9553612873278663</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="20.399999999999999">
+    <row r="27" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A27" s="8" t="s">
         <v>7</v>
       </c>
@@ -1571,7 +1577,7 @@
         <v>1.6056343167843523</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="20.399999999999999">
+    <row r="28" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A28" s="8" t="s">
         <v>7</v>
       </c>
@@ -1600,7 +1606,7 @@
         <v>1.9427727583085888</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="20.399999999999999">
+    <row r="29" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A29" s="8" t="s">
         <v>7</v>
       </c>
@@ -1629,7 +1635,7 @@
         <v>1.8139157885755728</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="20.399999999999999">
+    <row r="30" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A30" s="8" t="s">
         <v>7</v>
       </c>
@@ -1658,7 +1664,7 @@
         <v>2.029557740917729</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="20.399999999999999">
+    <row r="31" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A31" s="8" t="s">
         <v>7</v>
       </c>
@@ -1687,7 +1693,7 @@
         <v>1.903173090017704</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="20.399999999999999">
+    <row r="32" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A32" s="8" t="s">
         <v>8</v>
       </c>
@@ -1716,7 +1722,7 @@
         <v>1.9927617509384301</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="20.399999999999999">
+    <row r="33" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A33" s="8" t="s">
         <v>8</v>
       </c>
@@ -1745,7 +1751,7 @@
         <v>1.5323381652247765</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="20.399999999999999">
+    <row r="34" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A34" s="7" t="s">
         <v>9</v>
       </c>
@@ -1774,7 +1780,7 @@
         <v>2.3725059425196284</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="20.399999999999999">
+    <row r="35" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A35" s="9" t="s">
         <v>9</v>
       </c>
@@ -1803,7 +1809,7 @@
         <v>1.4157973174366616</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="20.399999999999999">
+    <row r="36" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A36" s="9" t="s">
         <v>9</v>
       </c>
@@ -1832,7 +1838,7 @@
         <v>1.7586950568259618</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="20.399999999999999">
+    <row r="37" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A37" s="9" t="s">
         <v>9</v>
       </c>
@@ -1861,7 +1867,7 @@
         <v>1.0846254578580783</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="20.399999999999999">
+    <row r="38" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A38" s="9" t="s">
         <v>9</v>
       </c>
@@ -1890,7 +1896,7 @@
         <v>1.4489633702060012</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="20.399999999999999">
+    <row r="39" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A39" s="8" t="s">
         <v>10</v>
       </c>
@@ -1919,7 +1925,7 @@
         <v>0.9354072919250257</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="20.399999999999999">
+    <row r="40" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A40" s="8" t="s">
         <v>10</v>
       </c>
@@ -1948,7 +1954,7 @@
         <v>0.60476092203608822</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="20.399999999999999">
+    <row r="41" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A41" s="8" t="s">
         <v>10</v>
       </c>
@@ -1977,7 +1983,7 @@
         <v>0.99056075812409061</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="20.399999999999999">
+    <row r="42" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A42" s="8" t="s">
         <v>10</v>
       </c>
@@ -2006,7 +2012,7 @@
         <v>0.88828499066422639</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="20.399999999999999">
+    <row r="43" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A43" s="8" t="s">
         <v>10</v>
       </c>
@@ -2035,7 +2041,7 @@
         <v>1.2386965594734871</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="20.399999999999999">
+    <row r="44" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A44" s="8" t="s">
         <v>11</v>
       </c>
@@ -2064,7 +2070,7 @@
         <v>1.771259342828938</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="20.399999999999999">
+    <row r="45" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A45" s="8" t="s">
         <v>11</v>
       </c>
@@ -2093,7 +2099,7 @@
         <v>1.3424908252120342</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="20.399999999999999">
+    <row r="46" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A46" s="8" t="s">
         <v>11</v>
       </c>
@@ -2122,7 +2128,7 @@
         <v>1.1832908136809575</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="20.399999999999999">
+    <row r="47" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A47" s="8" t="s">
         <v>11</v>
       </c>
@@ -2151,7 +2157,7 @@
         <v>1.0582010582010581</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="20.399999999999999">
+    <row r="48" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A48" s="8" t="s">
         <v>12</v>
       </c>
@@ -2180,7 +2186,7 @@
         <v>1.9507453556674683</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="20.399999999999999">
+    <row r="49" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A49" s="8" t="s">
         <v>12</v>
       </c>
@@ -2209,7 +2215,7 @@
         <v>1.3564734915079275</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="20.399999999999999">
+    <row r="50" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A50" s="8" t="s">
         <v>12</v>
       </c>
@@ -2238,7 +2244,7 @@
         <v>0.91394554845487175</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="20.399999999999999">
+    <row r="51" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A51" s="8" t="s">
         <v>12</v>
       </c>
@@ -2267,7 +2273,7 @@
         <v>1.0651127170937387</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="20.399999999999999">
+    <row r="52" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A52" s="8" t="s">
         <v>12</v>
       </c>
@@ -2296,7 +2302,7 @@
         <v>0.7190007334474251</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="20.399999999999999">
+    <row r="53" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A53" s="8" t="s">
         <v>12</v>
       </c>
@@ -2325,7 +2331,7 @@
         <v>1.2421910553969633</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="20.399999999999999">
+    <row r="54" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A54" s="8" t="s">
         <v>12</v>
       </c>
@@ -2354,7 +2360,7 @@
         <v>0.8564003829603678</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="20.399999999999999">
+    <row r="55" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A55" s="8" t="s">
         <v>12</v>
       </c>
@@ -2383,7 +2389,7 @@
         <v>0.70517723733981574</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="20.399999999999999">
+    <row r="56" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A56" s="8" t="s">
         <v>12</v>
       </c>
@@ -2412,7 +2418,7 @@
         <v>0.70133535989577678</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="20.399999999999999">
+    <row r="57" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A57" s="8" t="s">
         <v>12</v>
       </c>
@@ -2441,7 +2447,7 @@
         <v>0.5878578377595165</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="20.399999999999999">
+    <row r="58" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A58" s="8" t="s">
         <v>13</v>
       </c>
@@ -2470,7 +2476,7 @@
         <v>2.2687609075043631</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="20.399999999999999">
+    <row r="59" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A59" s="8" t="s">
         <v>13</v>
       </c>
@@ -2499,7 +2505,7 @@
         <v>2.3362599183060238</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="20.399999999999999">
+    <row r="60" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A60" s="8" t="s">
         <v>13</v>
       </c>
@@ -2528,7 +2534,7 @@
         <v>2.1263580518149001</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="20.399999999999999">
+    <row r="61" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A61" s="8" t="s">
         <v>14</v>
       </c>
@@ -2557,7 +2563,7 @@
         <v>1.8608527811896824</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="20.399999999999999">
+    <row r="62" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A62" s="8" t="s">
         <v>14</v>
       </c>
@@ -2586,7 +2592,7 @@
         <v>1.236697280332868</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="20.399999999999999">
+    <row r="63" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A63" s="8" t="s">
         <v>14</v>
       </c>
@@ -2615,7 +2621,7 @@
         <v>1.3316748371990927</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="20.399999999999999">
+    <row r="64" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A64" s="8" t="s">
         <v>14</v>
       </c>
@@ -2644,7 +2650,7 @@
         <v>1.9669558245263867</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="20.399999999999999">
+    <row r="65" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A65" s="8" t="s">
         <v>15</v>
       </c>
@@ -2673,7 +2679,7 @@
         <v>2.3846434047455674</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="20.399999999999999">
+    <row r="66" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A66" s="8" t="s">
         <v>15</v>
       </c>
@@ -2702,7 +2708,7 @@
         <v>1.6514536412139391</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="20.399999999999999">
+    <row r="67" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A67" s="8" t="s">
         <v>15</v>
       </c>
@@ -2731,7 +2737,7 @@
         <v>1.3600887933616392</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="20.399999999999999">
+    <row r="68" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A68" s="8" t="s">
         <v>15</v>
       </c>
@@ -2760,7 +2766,7 @@
         <v>1.6792916871618297</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="20.399999999999999">
+    <row r="69" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A69" s="8" t="s">
         <v>15</v>
       </c>
@@ -2789,7 +2795,7 @@
         <v>1.9190365113239698</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="20.399999999999999">
+    <row r="70" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A70" s="8" t="s">
         <v>15</v>
       </c>
@@ -2818,7 +2824,7 @@
         <v>1.6756659637443381</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="20.399999999999999">
+    <row r="71" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A71" s="9" t="s">
         <v>15</v>
       </c>
@@ -2847,7 +2853,7 @@
         <v>1.6878721672449986</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="20.399999999999999">
+    <row r="72" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A72" s="9" t="s">
         <v>15</v>
       </c>
@@ -2876,7 +2882,7 @@
         <v>3.3053544302393916</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="20.399999999999999">
+    <row r="73" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A73" s="8" t="s">
         <v>16</v>
       </c>
@@ -2905,7 +2911,7 @@
         <v>1.6892972407175879</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="20.399999999999999">
+    <row r="74" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A74" s="8" t="s">
         <v>16</v>
       </c>
@@ -2934,7 +2940,7 @@
         <v>1.4104303993796046</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="20.399999999999999">
+    <row r="75" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A75" s="8" t="s">
         <v>17</v>
       </c>
@@ -2963,7 +2969,7 @@
         <v>1.642896832746805</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="20.399999999999999">
+    <row r="76" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A76" s="8" t="s">
         <v>17</v>
       </c>
@@ -2992,7 +2998,7 @@
         <v>0.84051880298529091</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="20.399999999999999">
+    <row r="77" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A77" s="8" t="s">
         <v>17</v>
       </c>
@@ -3021,7 +3027,7 @@
         <v>0.89800943074775497</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="20.399999999999999">
+    <row r="78" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A78" s="8" t="s">
         <v>17</v>
       </c>
@@ -3050,7 +3056,7 @@
         <v>0.84955843619273874</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="20.399999999999999">
+    <row r="79" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A79" s="8" t="s">
         <v>17</v>
       </c>
@@ -3079,7 +3085,7 @@
         <v>0.80058086904043457</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="20.399999999999999">
+    <row r="80" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A80" s="8" t="s">
         <v>17</v>
       </c>
@@ -3108,7 +3114,7 @@
         <v>0.81071982944025733</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="20.399999999999999">
+    <row r="81" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A81" s="8" t="s">
         <v>18</v>
       </c>
@@ -3137,7 +3143,7 @@
         <v>2.2748316293213517</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="20.399999999999999">
+    <row r="82" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A82" s="8" t="s">
         <v>18</v>
       </c>
@@ -3166,7 +3172,7 @@
         <v>1.9743950128598611</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="20.399999999999999">
+    <row r="83" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A83" s="8" t="s">
         <v>18</v>
       </c>
@@ -3195,7 +3201,7 @@
         <v>1.9195639509049796</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="20.399999999999999">
+    <row r="84" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A84" s="8" t="s">
         <v>19</v>
       </c>
@@ -3224,7 +3230,7 @@
         <v>1.6618719101751249</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="20.399999999999999">
+    <row r="85" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A85" s="8" t="s">
         <v>19</v>
       </c>
@@ -3253,7 +3259,7 @@
         <v>1.13910443446762</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="20.399999999999999">
+    <row r="86" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A86" s="8" t="s">
         <v>19</v>
       </c>
@@ -3282,7 +3288,7 @@
         <v>1.2594816555576929</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="20.399999999999999">
+    <row r="87" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A87" s="8" t="s">
         <v>19</v>
       </c>
@@ -3311,7 +3317,7 @@
         <v>0.99357002604013045</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="20.399999999999999">
+    <row r="88" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A88" s="8" t="s">
         <v>19</v>
       </c>
@@ -3340,7 +3346,7 @@
         <v>1.0953980040675402</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="20.399999999999999">
+    <row r="89" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A89" s="8" t="s">
         <v>19</v>
       </c>
@@ -3369,7 +3375,7 @@
         <v>1.4138145612943374</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="20.399999999999999">
+    <row r="90" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A90" s="8" t="s">
         <v>19</v>
       </c>
@@ -3659,7 +3665,7 @@
         <v>0.79618629261718166</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="20.399999999999999">
+    <row r="100" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A100" s="8" t="s">
         <v>21</v>
       </c>
@@ -3688,7 +3694,7 @@
         <v>3.3645715636100464</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="20.399999999999999">
+    <row r="101" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A101" s="8" t="s">
         <v>21</v>
       </c>
@@ -3717,7 +3723,7 @@
         <v>2.3294819232202757</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="20.399999999999999">
+    <row r="102" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A102" s="8" t="s">
         <v>21</v>
       </c>
@@ -3746,7 +3752,7 @@
         <v>2.5410278141613376</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="20.399999999999999">
+    <row r="103" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A103" s="7" t="s">
         <v>22</v>
       </c>
@@ -3775,7 +3781,7 @@
         <v>1.9064519421782862</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="20.399999999999999">
+    <row r="104" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A104" s="9" t="s">
         <v>23</v>
       </c>
@@ -3804,7 +3810,7 @@
         <v>2.6629725653669531</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="20.399999999999999">
+    <row r="105" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A105" s="9" t="s">
         <v>23</v>
       </c>
@@ -3833,7 +3839,7 @@
         <v>1.8498489122799193</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="20.399999999999999">
+    <row r="106" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A106" s="9" t="s">
         <v>23</v>
       </c>
@@ -3862,7 +3868,7 @@
         <v>1.2042226573930268</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="20.399999999999999">
+    <row r="107" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A107" s="7" t="s">
         <v>24</v>
       </c>
@@ -3891,7 +3897,7 @@
         <v>2.2679929338913616</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="20.399999999999999">
+    <row r="108" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A108" s="9" t="s">
         <v>25</v>
       </c>
@@ -3920,7 +3926,7 @@
         <v>2.6287405400105186</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="20.399999999999999">
+    <row r="109" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A109" s="9" t="s">
         <v>25</v>
       </c>
@@ -3949,7 +3955,7 @@
         <v>1.1866477201904619</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="20.399999999999999">
+    <row r="110" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A110" s="9" t="s">
         <v>25</v>
       </c>
@@ -3978,7 +3984,7 @@
         <v>2.2032362231744553</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="20.399999999999999">
+    <row r="111" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A111" s="9" t="s">
         <v>25</v>
       </c>
@@ -4007,7 +4013,7 @@
         <v>2.2957652264892028</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="20.399999999999999">
+    <row r="112" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A112" s="9" t="s">
         <v>25</v>
       </c>
@@ -4036,7 +4042,7 @@
         <v>2.1891852232290252</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="20.399999999999999">
+    <row r="113" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A113" s="8" t="s">
         <v>26</v>
       </c>
@@ -4065,7 +4071,7 @@
         <v>0.4770783637670441</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="20.399999999999999">
+    <row r="114" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A114" s="8" t="s">
         <v>26</v>
       </c>
@@ -4094,7 +4100,7 @@
         <v>0.94120599861956455</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="20.399999999999999">
+    <row r="115" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A115" s="8" t="s">
         <v>26</v>
       </c>
@@ -4123,7 +4129,7 @@
         <v>0.81590596052949771</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="20.399999999999999">
+    <row r="116" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A116" s="8" t="s">
         <v>26</v>
       </c>
@@ -4152,7 +4158,7 @@
         <v>0.76325572701406053</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="20.399999999999999">
+    <row r="117" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A117" s="8" t="s">
         <v>27</v>
       </c>
@@ -4181,7 +4187,7 @@
         <v>2.7039041866059987</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="20.399999999999999">
+    <row r="118" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A118" s="8" t="s">
         <v>27</v>
       </c>
@@ -4210,7 +4216,7 @@
         <v>2.8341255135744783</v>
       </c>
     </row>
-    <row r="119" spans="1:9" ht="20.399999999999999">
+    <row r="119" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A119" s="8" t="s">
         <v>27</v>
       </c>
@@ -4239,7 +4245,7 @@
         <v>1.315647130291506</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="20.399999999999999">
+    <row r="120" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A120" s="8" t="s">
         <v>27</v>
       </c>
@@ -4268,7 +4274,7 @@
         <v>1.2227959015009464</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="20.399999999999999">
+    <row r="121" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A121" s="8" t="s">
         <v>27</v>
       </c>
@@ -4297,7 +4303,7 @@
         <v>1.1119391277063069</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="20.399999999999999">
+    <row r="122" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A122" s="8" t="s">
         <v>27</v>
       </c>
@@ -4326,7 +4332,7 @@
         <v>0.91111399403235305</v>
       </c>
     </row>
-    <row r="123" spans="1:9" ht="20.399999999999999">
+    <row r="123" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A123" s="8" t="s">
         <v>27</v>
       </c>
@@ -4355,7 +4361,7 @@
         <v>1.0627515983897704</v>
       </c>
     </row>
-    <row r="124" spans="1:9" ht="20.399999999999999">
+    <row r="124" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A124" s="8" t="s">
         <v>27</v>
       </c>
@@ -4384,7 +4390,7 @@
         <v>1.1867313530021368</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="20.399999999999999">
+    <row r="125" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A125" s="8" t="s">
         <v>27</v>
       </c>
@@ -4413,7 +4419,7 @@
         <v>1.861699900340851</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="20.399999999999999">
+    <row r="126" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A126" s="8" t="s">
         <v>27</v>
       </c>
@@ -4442,7 +4448,7 @@
         <v>0.968044779820739</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="20.399999999999999">
+    <row r="127" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A127" s="8" t="s">
         <v>27</v>
       </c>
@@ -4471,7 +4477,7 @@
         <v>1.4151228309359656</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="20.399999999999999">
+    <row r="128" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A128" s="8" t="s">
         <v>27</v>
       </c>
@@ -4500,7 +4506,7 @@
         <v>1.8304182228303072</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="20.399999999999999">
+    <row r="129" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A129" s="8" t="s">
         <v>27</v>
       </c>
@@ -4529,7 +4535,7 @@
         <v>0.84869719028505342</v>
       </c>
     </row>
-    <row r="130" spans="1:9" ht="20.399999999999999">
+    <row r="130" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A130" s="8" t="s">
         <v>27</v>
       </c>
@@ -4558,7 +4564,7 @@
         <v>1.0550246533279533</v>
       </c>
     </row>
-    <row r="131" spans="1:9" ht="20.399999999999999">
+    <row r="131" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A131" s="8" t="s">
         <v>28</v>
       </c>
@@ -4587,7 +4593,7 @@
         <v>2.3524895810484754</v>
       </c>
     </row>
-    <row r="132" spans="1:9" ht="20.399999999999999">
+    <row r="132" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A132" s="8" t="s">
         <v>28</v>
       </c>
@@ -4616,7 +4622,7 @@
         <v>1.3086111921624799</v>
       </c>
     </row>
-    <row r="133" spans="1:9" ht="20.399999999999999">
+    <row r="133" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A133" s="8" t="s">
         <v>28</v>
       </c>
@@ -4645,7 +4651,7 @@
         <v>2.1503751377875759</v>
       </c>
     </row>
-    <row r="134" spans="1:9" ht="20.399999999999999">
+    <row r="134" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A134" s="8" t="s">
         <v>28</v>
       </c>
@@ -4674,7 +4680,7 @@
         <v>2.9218293335528753</v>
       </c>
     </row>
-    <row r="135" spans="1:9" ht="20.399999999999999">
+    <row r="135" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A135" s="8" t="s">
         <v>28</v>
       </c>
@@ -4703,7 +4709,7 @@
         <v>2.1481802349737888</v>
       </c>
     </row>
-    <row r="136" spans="1:9" ht="20.399999999999999">
+    <row r="136" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A136" s="8" t="s">
         <v>28</v>
       </c>
@@ -4732,7 +4738,7 @@
         <v>2.594837175405623</v>
       </c>
     </row>
-    <row r="137" spans="1:9" ht="20.399999999999999">
+    <row r="137" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A137" s="8" t="s">
         <v>28</v>
       </c>
@@ -4761,7 +4767,7 @@
         <v>2.4045171932495877</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="20.399999999999999">
+    <row r="138" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A138" s="8" t="s">
         <v>28</v>
       </c>
@@ -4790,7 +4796,7 @@
         <v>1.8140003387322501</v>
       </c>
     </row>
-    <row r="139" spans="1:9" ht="20.399999999999999">
+    <row r="139" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A139" s="8" t="s">
         <v>29</v>
       </c>
@@ -4819,7 +4825,7 @@
         <v>2.0109912860181054</v>
       </c>
     </row>
-    <row r="140" spans="1:9" ht="20.399999999999999">
+    <row r="140" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A140" s="8" t="s">
         <v>29</v>
       </c>
@@ -4848,7 +4854,7 @@
         <v>1.6206639145958683</v>
       </c>
     </row>
-    <row r="141" spans="1:9" ht="20.399999999999999">
+    <row r="141" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A141" s="8" t="s">
         <v>29</v>
       </c>
@@ -4877,7 +4883,7 @@
         <v>1.0474631751227497</v>
       </c>
     </row>
-    <row r="142" spans="1:9" ht="20.399999999999999">
+    <row r="142" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A142" s="8" t="s">
         <v>29</v>
       </c>
@@ -4906,7 +4912,7 @@
         <v>1.0110374845075096</v>
       </c>
     </row>
-    <row r="143" spans="1:9" ht="20.399999999999999">
+    <row r="143" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A143" s="9" t="s">
         <v>29</v>
       </c>
@@ -4935,7 +4941,7 @@
         <v>1.6089759822350351</v>
       </c>
     </row>
-    <row r="144" spans="1:9" ht="20.399999999999999">
+    <row r="144" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A144" s="9" t="s">
         <v>29</v>
       </c>
@@ -4964,7 +4970,7 @@
         <v>0.87356663868136075</v>
       </c>
     </row>
-    <row r="145" spans="1:9" ht="20.399999999999999">
+    <row r="145" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A145" s="8" t="s">
         <v>30</v>
       </c>
@@ -4993,7 +4999,7 @@
         <v>2.0630040207215936</v>
       </c>
     </row>
-    <row r="146" spans="1:9" ht="20.399999999999999">
+    <row r="146" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A146" s="8" t="s">
         <v>30</v>
       </c>
@@ -5022,7 +5028,7 @@
         <v>2.2449690739611463</v>
       </c>
     </row>
-    <row r="147" spans="1:9" ht="20.399999999999999">
+    <row r="147" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A147" s="8" t="s">
         <v>30</v>
       </c>
@@ -5051,7 +5057,7 @@
         <v>2.2520450861386512</v>
       </c>
     </row>
-    <row r="148" spans="1:9" ht="20.399999999999999">
+    <row r="148" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A148" s="8" t="s">
         <v>30</v>
       </c>
@@ -5080,7 +5086,7 @@
         <v>2.1691470635301648</v>
       </c>
     </row>
-    <row r="149" spans="1:9" ht="20.399999999999999">
+    <row r="149" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A149" s="8" t="s">
         <v>30</v>
       </c>
@@ -5109,7 +5115,7 @@
         <v>2.6213892405995112</v>
       </c>
     </row>
-    <row r="150" spans="1:9" ht="20.399999999999999">
+    <row r="150" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A150" s="8" t="s">
         <v>30</v>
       </c>
@@ -5138,7 +5144,7 @@
         <v>1.9718957630111449</v>
       </c>
     </row>
-    <row r="151" spans="1:9" ht="20.399999999999999">
+    <row r="151" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A151" s="8" t="s">
         <v>31</v>
       </c>
@@ -5167,7 +5173,7 @@
         <v>1.6430516453593023</v>
       </c>
     </row>
-    <row r="152" spans="1:9" ht="20.399999999999999">
+    <row r="152" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A152" s="8" t="s">
         <v>31</v>
       </c>
@@ -5196,7 +5202,7 @@
         <v>1.2509212797964602</v>
       </c>
     </row>
-    <row r="153" spans="1:9" ht="20.399999999999999">
+    <row r="153" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A153" s="8" t="s">
         <v>31</v>
       </c>
@@ -5225,7 +5231,7 @@
         <v>0.98605278944211161</v>
       </c>
     </row>
-    <row r="154" spans="1:9" ht="20.399999999999999">
+    <row r="154" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A154" s="8" t="s">
         <v>31</v>
       </c>
@@ -5254,7 +5260,7 @@
         <v>0.72004679480314049</v>
       </c>
     </row>
-    <row r="155" spans="1:9" ht="20.399999999999999">
+    <row r="155" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A155" s="8" t="s">
         <v>32</v>
       </c>
@@ -5283,7 +5289,7 @@
         <v>1.941315681773697</v>
       </c>
     </row>
-    <row r="156" spans="1:9" ht="20.399999999999999">
+    <row r="156" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A156" s="8" t="s">
         <v>32</v>
       </c>
@@ -5312,7 +5318,7 @@
         <v>1.2701425435443208</v>
       </c>
     </row>
-    <row r="157" spans="1:9" ht="20.399999999999999">
+    <row r="157" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A157" s="8" t="s">
         <v>32</v>
       </c>
@@ -5341,7 +5347,7 @@
         <v>1.1470415308140467</v>
       </c>
     </row>
-    <row r="158" spans="1:9" ht="20.399999999999999">
+    <row r="158" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A158" s="8" t="s">
         <v>33</v>
       </c>
@@ -5370,7 +5376,7 @@
         <v>0.68868091117782093</v>
       </c>
     </row>
-    <row r="159" spans="1:9" ht="20.399999999999999">
+    <row r="159" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A159" s="8" t="s">
         <v>33</v>
       </c>
@@ -5399,7 +5405,7 @@
         <v>0.75186596139264217</v>
       </c>
     </row>
-    <row r="160" spans="1:9" ht="20.399999999999999">
+    <row r="160" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A160" s="8" t="s">
         <v>34</v>
       </c>
@@ -5428,7 +5434,7 @@
         <v>1.9732888446393815</v>
       </c>
     </row>
-    <row r="161" spans="1:9" ht="20.399999999999999">
+    <row r="161" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A161" s="8" t="s">
         <v>34</v>
       </c>
@@ -5457,7 +5463,7 @@
         <v>0.84254662684677917</v>
       </c>
     </row>
-    <row r="162" spans="1:9" ht="20.399999999999999">
+    <row r="162" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A162" s="8" t="s">
         <v>34</v>
       </c>
@@ -5486,7 +5492,7 @@
         <v>0.84649039376070001</v>
       </c>
     </row>
-    <row r="163" spans="1:9" ht="20.399999999999999">
+    <row r="163" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A163" s="8" t="s">
         <v>34</v>
       </c>
@@ -5515,7 +5521,7 @@
         <v>0.83483628655894981</v>
       </c>
     </row>
-    <row r="164" spans="1:9" ht="20.399999999999999">
+    <row r="164" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A164" s="8" t="s">
         <v>34</v>
       </c>
@@ -5544,7 +5550,7 @@
         <v>1.0175046116409592</v>
       </c>
     </row>
-    <row r="165" spans="1:9" ht="20.399999999999999">
+    <row r="165" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A165" s="8" t="s">
         <v>34</v>
       </c>
@@ -5573,7 +5579,7 @@
         <v>1.2477416943299842</v>
       </c>
     </row>
-    <row r="166" spans="1:9" ht="20.399999999999999">
+    <row r="166" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A166" s="8" t="s">
         <v>34</v>
       </c>
@@ -5602,7 +5608,7 @@
         <v>1.1194628087482199</v>
       </c>
     </row>
-    <row r="167" spans="1:9" ht="20.399999999999999">
+    <row r="167" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A167" s="8" t="s">
         <v>34</v>
       </c>
@@ -5631,7 +5637,7 @@
         <v>4.059851417808936</v>
       </c>
     </row>
-    <row r="168" spans="1:9" ht="20.399999999999999">
+    <row r="168" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A168" s="8" t="s">
         <v>35</v>
       </c>
@@ -5660,7 +5666,7 @@
         <v>1.9483218454504521</v>
       </c>
     </row>
-    <row r="169" spans="1:9" ht="20.399999999999999">
+    <row r="169" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A169" s="8" t="s">
         <v>35</v>
       </c>
@@ -5689,7 +5695,7 @@
         <v>1.9251087761333101</v>
       </c>
     </row>
-    <row r="170" spans="1:9" ht="20.399999999999999">
+    <row r="170" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A170" s="8" t="s">
         <v>35</v>
       </c>
@@ -5718,7 +5724,7 @@
         <v>1.7377386532525436</v>
       </c>
     </row>
-    <row r="171" spans="1:9" ht="20.399999999999999">
+    <row r="171" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A171" s="8" t="s">
         <v>35</v>
       </c>
@@ -5747,7 +5753,7 @@
         <v>1.8251564357810506</v>
       </c>
     </row>
-    <row r="172" spans="1:9" ht="20.399999999999999">
+    <row r="172" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A172" s="8" t="s">
         <v>35</v>
       </c>
@@ -5776,7 +5782,7 @@
         <v>1.8795180722891567</v>
       </c>
     </row>
-    <row r="173" spans="1:9" ht="20.399999999999999">
+    <row r="173" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A173" s="8" t="s">
         <v>35</v>
       </c>
@@ -5805,7 +5811,7 @@
         <v>1.268329526195564</v>
       </c>
     </row>
-    <row r="174" spans="1:9" ht="20.399999999999999">
+    <row r="174" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A174" s="8" t="s">
         <v>36</v>
       </c>
@@ -5834,7 +5840,7 @@
         <v>1.7163877966610674</v>
       </c>
     </row>
-    <row r="175" spans="1:9" ht="20.399999999999999">
+    <row r="175" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A175" s="8" t="s">
         <v>36</v>
       </c>
@@ -5863,7 +5869,7 @@
         <v>1.8904709545677141</v>
       </c>
     </row>
-    <row r="176" spans="1:9" ht="20.399999999999999">
+    <row r="176" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A176" s="8" t="s">
         <v>36</v>
       </c>
@@ -5892,7 +5898,7 @@
         <v>1.2903090447516943</v>
       </c>
     </row>
-    <row r="177" spans="1:9" ht="20.399999999999999">
+    <row r="177" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A177" s="8" t="s">
         <v>37</v>
       </c>
@@ -5921,7 +5927,7 @@
         <v>1.9055300210861812</v>
       </c>
     </row>
-    <row r="178" spans="1:9" ht="20.399999999999999">
+    <row r="178" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A178" s="8" t="s">
         <v>37</v>
       </c>
@@ -5950,7 +5956,7 @@
         <v>1.4520626983363785</v>
       </c>
     </row>
-    <row r="179" spans="1:9" ht="20.399999999999999">
+    <row r="179" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A179" s="7" t="s">
         <v>37</v>
       </c>
@@ -5979,7 +5985,7 @@
         <v>1.3280115352064112</v>
       </c>
     </row>
-    <row r="180" spans="1:9" ht="20.399999999999999">
+    <row r="180" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A180" s="8" t="s">
         <v>38</v>
       </c>
@@ -6008,7 +6014,7 @@
         <v>1.162556473195016</v>
       </c>
     </row>
-    <row r="181" spans="1:9" ht="20.399999999999999">
+    <row r="181" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A181" s="8" t="s">
         <v>38</v>
       </c>
@@ -6037,7 +6043,7 @@
         <v>1.34942414486052</v>
       </c>
     </row>
-    <row r="182" spans="1:9" ht="20.399999999999999">
+    <row r="182" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A182" s="8" t="s">
         <v>38</v>
       </c>
@@ -6066,7 +6072,7 @@
         <v>0.93329673346143294</v>
       </c>
     </row>
-    <row r="183" spans="1:9" ht="20.399999999999999">
+    <row r="183" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A183" s="8" t="s">
         <v>38</v>
       </c>
@@ -6095,7 +6101,7 @@
         <v>0.53563086016014605</v>
       </c>
     </row>
-    <row r="184" spans="1:9" ht="20.399999999999999">
+    <row r="184" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A184" s="8" t="s">
         <v>39</v>
       </c>
@@ -6124,7 +6130,7 @@
         <v>2.8478251662360763</v>
       </c>
     </row>
-    <row r="185" spans="1:9" ht="20.399999999999999">
+    <row r="185" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A185" s="8" t="s">
         <v>39</v>
       </c>
@@ -6153,7 +6159,7 @@
         <v>1.7186479754294606</v>
       </c>
     </row>
-    <row r="186" spans="1:9" ht="20.399999999999999">
+    <row r="186" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A186" s="8" t="s">
         <v>39</v>
       </c>
@@ -6182,7 +6188,7 @@
         <v>1.3385057891205718</v>
       </c>
     </row>
-    <row r="187" spans="1:9" ht="20.399999999999999">
+    <row r="187" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A187" s="8" t="s">
         <v>39</v>
       </c>
@@ -6211,7 +6217,7 @@
         <v>1.6556001052186875</v>
       </c>
     </row>
-    <row r="188" spans="1:9" ht="20.399999999999999">
+    <row r="188" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A188" s="8" t="s">
         <v>40</v>
       </c>
@@ -6240,7 +6246,7 @@
         <v>1.5838011226944668</v>
       </c>
     </row>
-    <row r="189" spans="1:9" ht="20.399999999999999">
+    <row r="189" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A189" s="8" t="s">
         <v>40</v>
       </c>
@@ -6269,7 +6275,7 @@
         <v>1.3472617407828194</v>
       </c>
     </row>
-    <row r="190" spans="1:9" ht="20.399999999999999">
+    <row r="190" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A190" s="8" t="s">
         <v>40</v>
       </c>
@@ -6298,7 +6304,7 @@
         <v>1.2681142069018361</v>
       </c>
     </row>
-    <row r="191" spans="1:9" ht="20.399999999999999">
+    <row r="191" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A191" s="7" t="s">
         <v>41</v>
       </c>
@@ -6327,7 +6333,7 @@
         <v>2.3655582922824303</v>
       </c>
     </row>
-    <row r="192" spans="1:9" ht="20.399999999999999">
+    <row r="192" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A192" s="9" t="s">
         <v>42</v>
       </c>
@@ -6356,7 +6362,7 @@
         <v>2.0330018456791823</v>
       </c>
     </row>
-    <row r="193" spans="1:9" ht="20.399999999999999">
+    <row r="193" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A193" s="9" t="s">
         <v>42</v>
       </c>
@@ -6385,7 +6391,7 @@
         <v>1.9072025896951712</v>
       </c>
     </row>
-    <row r="194" spans="1:9" ht="20.399999999999999">
+    <row r="194" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A194" s="9" t="s">
         <v>42</v>
       </c>
@@ -6414,7 +6420,7 @@
         <v>1.8495960223741454</v>
       </c>
     </row>
-    <row r="195" spans="1:9" ht="20.399999999999999">
+    <row r="195" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A195" s="8" t="s">
         <v>43</v>
       </c>
@@ -6443,7 +6449,7 @@
         <v>1.5442244476721962</v>
       </c>
     </row>
-    <row r="196" spans="1:9" ht="20.399999999999999">
+    <row r="196" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A196" s="8" t="s">
         <v>43</v>
       </c>
@@ -6472,7 +6478,7 @@
         <v>1.3860671376269789</v>
       </c>
     </row>
-    <row r="197" spans="1:9" ht="20.399999999999999">
+    <row r="197" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A197" s="8" t="s">
         <v>43</v>
       </c>
@@ -6501,7 +6507,7 @@
         <v>0.92390669418591065</v>
       </c>
     </row>
-    <row r="198" spans="1:9" ht="20.399999999999999">
+    <row r="198" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A198" s="8" t="s">
         <v>44</v>
       </c>
@@ -6530,7 +6536,7 @@
         <v>3.1142865374088906</v>
       </c>
     </row>
-    <row r="199" spans="1:9" ht="20.399999999999999">
+    <row r="199" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A199" s="8" t="s">
         <v>44</v>
       </c>
@@ -6559,7 +6565,7 @@
         <v>1.9407596189987257</v>
       </c>
     </row>
-    <row r="200" spans="1:9" ht="20.399999999999999">
+    <row r="200" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A200" s="8" t="s">
         <v>44</v>
       </c>
@@ -6588,7 +6594,7 @@
         <v>1.6820814600672833</v>
       </c>
     </row>
-    <row r="201" spans="1:9" ht="20.399999999999999">
+    <row r="201" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A201" s="8" t="s">
         <v>44</v>
       </c>
@@ -6617,7 +6623,7 @@
         <v>1.3352107683369929</v>
       </c>
     </row>
-    <row r="202" spans="1:9" ht="20.399999999999999">
+    <row r="202" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A202" s="8" t="s">
         <v>44</v>
       </c>
@@ -6646,7 +6652,7 @@
         <v>1.9717483846830541</v>
       </c>
     </row>
-    <row r="203" spans="1:9" ht="20.399999999999999">
+    <row r="203" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A203" s="8" t="s">
         <v>45</v>
       </c>
@@ -6675,7 +6681,7 @@
         <v>2.1555943526657315</v>
       </c>
     </row>
-    <row r="204" spans="1:9" ht="20.399999999999999">
+    <row r="204" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A204" s="8" t="s">
         <v>45</v>
       </c>
@@ -6704,7 +6710,7 @@
         <v>1.5965673330818559</v>
       </c>
     </row>
-    <row r="205" spans="1:9" ht="20.399999999999999">
+    <row r="205" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A205" s="8" t="s">
         <v>45</v>
       </c>
@@ -6733,7 +6739,7 @@
         <v>1.8074813347554473</v>
       </c>
     </row>
-    <row r="206" spans="1:9" ht="20.399999999999999">
+    <row r="206" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A206" s="8" t="s">
         <v>46</v>
       </c>
@@ -6762,7 +6768,7 @@
         <v>1.9386160068149301</v>
       </c>
     </row>
-    <row r="207" spans="1:9" ht="20.399999999999999">
+    <row r="207" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A207" s="8" t="s">
         <v>46</v>
       </c>
@@ -6791,7 +6797,7 @@
         <v>1.4300783483239257</v>
       </c>
     </row>
-    <row r="208" spans="1:9" ht="20.399999999999999">
+    <row r="208" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A208" s="8" t="s">
         <v>46</v>
       </c>
@@ -6820,7 +6826,7 @@
         <v>1.2767902109641678</v>
       </c>
     </row>
-    <row r="209" spans="1:9" ht="20.399999999999999">
+    <row r="209" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A209" s="8" t="s">
         <v>46</v>
       </c>
@@ -6849,7 +6855,7 @@
         <v>1.2645047512734162</v>
       </c>
     </row>
-    <row r="210" spans="1:9" ht="20.399999999999999">
+    <row r="210" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A210" s="8" t="s">
         <v>46</v>
       </c>
@@ -6878,7 +6884,7 @@
         <v>1.6574689695440077</v>
       </c>
     </row>
-    <row r="211" spans="1:9" ht="20.399999999999999">
+    <row r="211" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A211" s="8" t="s">
         <v>47</v>
       </c>
@@ -6907,7 +6913,7 @@
         <v>3.7845040928992955</v>
       </c>
     </row>
-    <row r="212" spans="1:9" ht="20.399999999999999">
+    <row r="212" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A212" s="8" t="s">
         <v>47</v>
       </c>
@@ -6936,7 +6942,7 @@
         <v>7.3657863819788529</v>
       </c>
     </row>
-    <row r="213" spans="1:9" ht="20.399999999999999">
+    <row r="213" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A213" s="10" t="s">
         <v>48</v>
       </c>
@@ -6965,7 +6971,7 @@
         <v>2.8614369644565025</v>
       </c>
     </row>
-    <row r="214" spans="1:9" ht="20.399999999999999">
+    <row r="214" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A214" s="10" t="s">
         <v>48</v>
       </c>
@@ -6994,7 +7000,7 @@
         <v>2.8755760368663594</v>
       </c>
     </row>
-    <row r="215" spans="1:9" ht="20.399999999999999">
+    <row r="215" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A215" s="9" t="s">
         <v>49</v>
       </c>
@@ -7023,7 +7029,7 @@
         <v>1.0958290473504331</v>
       </c>
     </row>
-    <row r="216" spans="1:9" ht="20.399999999999999">
+    <row r="216" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A216" s="9" t="s">
         <v>49</v>
       </c>
@@ -7052,7 +7058,7 @@
         <v>0.85269286209026751</v>
       </c>
     </row>
-    <row r="217" spans="1:9" ht="20.399999999999999">
+    <row r="217" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A217" s="9" t="s">
         <v>49</v>
       </c>
@@ -7081,7 +7087,7 @@
         <v>0.59408782167798713</v>
       </c>
     </row>
-    <row r="218" spans="1:9" ht="20.399999999999999">
+    <row r="218" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A218" s="9" t="s">
         <v>49</v>
       </c>
@@ -7110,7 +7116,7 @@
         <v>0.90222659591100973</v>
       </c>
     </row>
-    <row r="219" spans="1:9" ht="20.399999999999999">
+    <row r="219" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A219" s="9" t="s">
         <v>49</v>
       </c>
@@ -7139,7 +7145,7 @@
         <v>0.70148090413094311</v>
       </c>
     </row>
-    <row r="220" spans="1:9" ht="20.399999999999999">
+    <row r="220" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A220" s="8" t="s">
         <v>50</v>
       </c>
@@ -7168,7 +7174,7 @@
         <v>1.0135727221389208</v>
       </c>
     </row>
-    <row r="221" spans="1:9" ht="20.399999999999999">
+    <row r="221" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A221" s="8" t="s">
         <v>50</v>
       </c>
@@ -7197,7 +7203,7 @@
         <v>1.0683866864111151</v>
       </c>
     </row>
-    <row r="222" spans="1:9" ht="20.399999999999999">
+    <row r="222" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A222" s="7" t="s">
         <v>51</v>
       </c>
@@ -7226,7 +7232,7 @@
         <v>1.3010959869061678</v>
       </c>
     </row>
-    <row r="223" spans="1:9" ht="20.399999999999999">
+    <row r="223" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A223" s="9" t="s">
         <v>52</v>
       </c>
@@ -7255,7 +7261,7 @@
         <v>1.0160944105433856</v>
       </c>
     </row>
-    <row r="224" spans="1:9" ht="20.399999999999999">
+    <row r="224" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A224" s="9" t="s">
         <v>52</v>
       </c>
@@ -7284,7 +7290,7 @@
         <v>0.6036614508654905</v>
       </c>
     </row>
-    <row r="225" spans="1:9" ht="20.399999999999999">
+    <row r="225" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A225" s="9" t="s">
         <v>52</v>
       </c>
@@ -7313,7 +7319,7 @@
         <v>0.53817592921752178</v>
       </c>
     </row>
-    <row r="226" spans="1:9" ht="20.399999999999999">
+    <row r="226" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A226" s="8" t="s">
         <v>53</v>
       </c>
@@ -7342,7 +7348,7 @@
         <v>2.2657557891672124</v>
       </c>
     </row>
-    <row r="227" spans="1:9" ht="20.399999999999999">
+    <row r="227" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A227" s="8" t="s">
         <v>53</v>
       </c>
@@ -7371,7 +7377,7 @@
         <v>0.72298927879099573</v>
       </c>
     </row>
-    <row r="228" spans="1:9" ht="20.399999999999999">
+    <row r="228" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A228" s="8" t="s">
         <v>53</v>
       </c>
@@ -7400,7 +7406,7 @@
         <v>1.5647077293421947</v>
       </c>
     </row>
-    <row r="229" spans="1:9" ht="20.399999999999999">
+    <row r="229" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A229" s="8" t="s">
         <v>54</v>
       </c>
@@ -7429,7 +7435,7 @@
         <v>1.1020455834751559</v>
       </c>
     </row>
-    <row r="230" spans="1:9" ht="20.399999999999999">
+    <row r="230" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A230" s="8" t="s">
         <v>54</v>
       </c>
@@ -7458,7 +7464,7 @@
         <v>0.81105044565775353</v>
       </c>
     </row>
-    <row r="231" spans="1:9" ht="20.399999999999999">
+    <row r="231" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A231" s="8" t="s">
         <v>54</v>
       </c>
@@ -7487,7 +7493,7 @@
         <v>0.59191154377741717</v>
       </c>
     </row>
-    <row r="232" spans="1:9" ht="20.399999999999999">
+    <row r="232" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A232" s="8" t="s">
         <v>54</v>
       </c>
@@ -7516,7 +7522,7 @@
         <v>0.6561177182019754</v>
       </c>
     </row>
-    <row r="233" spans="1:9" ht="20.399999999999999">
+    <row r="233" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A233" s="8" t="s">
         <v>54</v>
       </c>
@@ -7545,7 +7551,7 @@
         <v>0.63598721860904761</v>
       </c>
     </row>
-    <row r="234" spans="1:9" ht="20.399999999999999">
+    <row r="234" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A234" s="8" t="s">
         <v>54</v>
       </c>
@@ -7574,7 +7580,7 @@
         <v>0.63168802184006534</v>
       </c>
     </row>
-    <row r="235" spans="1:9" ht="20.399999999999999">
+    <row r="235" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A235" s="8" t="s">
         <v>54</v>
       </c>
@@ -7603,7 +7609,7 @@
         <v>0.67052289274511501</v>
       </c>
     </row>
-    <row r="236" spans="1:9" ht="20.399999999999999">
+    <row r="236" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A236" s="7" t="s">
         <v>55</v>
       </c>
@@ -7632,7 +7638,7 @@
         <v>1.9624984038739208</v>
       </c>
     </row>
-    <row r="237" spans="1:9" ht="20.399999999999999">
+    <row r="237" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A237" s="9" t="s">
         <v>56</v>
       </c>
@@ -7661,7 +7667,7 @@
         <v>2.8891372656530083</v>
       </c>
     </row>
-    <row r="238" spans="1:9" ht="20.399999999999999">
+    <row r="238" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A238" s="9" t="s">
         <v>56</v>
       </c>
@@ -7690,7 +7696,7 @@
         <v>2.0254689544175366</v>
       </c>
     </row>
-    <row r="239" spans="1:9" ht="20.399999999999999">
+    <row r="239" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A239" s="9" t="s">
         <v>56</v>
       </c>
@@ -7719,7 +7725,7 @@
         <v>1.7749233965450182</v>
       </c>
     </row>
-    <row r="240" spans="1:9" ht="20.399999999999999">
+    <row r="240" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A240" s="9" t="s">
         <v>56</v>
       </c>
@@ -7748,7 +7754,7 @@
         <v>1.9206258087741659</v>
       </c>
     </row>
-    <row r="241" spans="1:9" ht="20.399999999999999">
+    <row r="241" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A241" s="8" t="s">
         <v>57</v>
       </c>
@@ -7777,7 +7783,7 @@
         <v>1.6950357130165949</v>
       </c>
     </row>
-    <row r="242" spans="1:9" ht="20.399999999999999">
+    <row r="242" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A242" s="8" t="s">
         <v>57</v>
       </c>
@@ -7806,7 +7812,7 @@
         <v>1.3523610970176103</v>
       </c>
     </row>
-    <row r="243" spans="1:9" ht="20.399999999999999">
+    <row r="243" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A243" s="8" t="s">
         <v>57</v>
       </c>
@@ -7835,7 +7841,7 @@
         <v>1.7786404340729631</v>
       </c>
     </row>
-    <row r="244" spans="1:9" ht="20.399999999999999">
+    <row r="244" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A244" s="8" t="s">
         <v>57</v>
       </c>
@@ -7864,7 +7870,7 @@
         <v>1.655412169418103</v>
       </c>
     </row>
-    <row r="245" spans="1:9" ht="20.399999999999999">
+    <row r="245" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A245" s="8" t="s">
         <v>57</v>
       </c>
@@ -7893,7 +7899,7 @@
         <v>2.1150347529971545</v>
       </c>
     </row>
-    <row r="246" spans="1:9" ht="20.399999999999999">
+    <row r="246" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A246" s="8" t="s">
         <v>58</v>
       </c>
@@ -7922,7 +7928,7 @@
         <v>3.044354138446042</v>
       </c>
     </row>
-    <row r="247" spans="1:9" ht="20.399999999999999">
+    <row r="247" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A247" s="8" t="s">
         <v>58</v>
       </c>
@@ -7951,7 +7957,7 @@
         <v>1.4527421236872813</v>
       </c>
     </row>
-    <row r="248" spans="1:9" ht="20.399999999999999">
+    <row r="248" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A248" s="8" t="s">
         <v>58</v>
       </c>
@@ -7980,7 +7986,7 @@
         <v>1.8363215731636784</v>
       </c>
     </row>
-    <row r="249" spans="1:9" ht="20.399999999999999">
+    <row r="249" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A249" s="8" t="s">
         <v>58</v>
       </c>
@@ -8009,7 +8015,7 @@
         <v>1.1557340473003124</v>
       </c>
     </row>
-    <row r="250" spans="1:9" ht="20.399999999999999">
+    <row r="250" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A250" s="7" t="s">
         <v>59</v>
       </c>
@@ -8038,7 +8044,7 @@
         <v>1.9856775900988557</v>
       </c>
     </row>
-    <row r="251" spans="1:9" ht="20.399999999999999">
+    <row r="251" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A251" s="9" t="s">
         <v>59</v>
       </c>
@@ -8067,7 +8073,7 @@
         <v>1.3164809519992162</v>
       </c>
     </row>
-    <row r="252" spans="1:9" ht="20.399999999999999">
+    <row r="252" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A252" s="9" t="s">
         <v>59</v>
       </c>
@@ -8096,7 +8102,7 @@
         <v>2.2044287033715242</v>
       </c>
     </row>
-    <row r="253" spans="1:9" ht="20.399999999999999">
+    <row r="253" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A253" s="9" t="s">
         <v>59</v>
       </c>
@@ -8125,7 +8131,7 @@
         <v>1.2314218332040709</v>
       </c>
     </row>
-    <row r="254" spans="1:9" ht="20.399999999999999">
+    <row r="254" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A254" s="8" t="s">
         <v>60</v>
       </c>
@@ -8154,7 +8160,7 @@
         <v>1.6344714864035421</v>
       </c>
     </row>
-    <row r="255" spans="1:9" ht="20.399999999999999">
+    <row r="255" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A255" s="8" t="s">
         <v>60</v>
       </c>
@@ -8183,7 +8189,7 @@
         <v>1.3411026691649337</v>
       </c>
     </row>
-    <row r="256" spans="1:9" ht="20.399999999999999">
+    <row r="256" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A256" s="8" t="s">
         <v>61</v>
       </c>
@@ -8212,7 +8218,7 @@
         <v>1.2910581130215073</v>
       </c>
     </row>
-    <row r="257" spans="1:9" ht="20.399999999999999">
+    <row r="257" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A257" s="8" t="s">
         <v>61</v>
       </c>
@@ -8241,7 +8247,7 @@
         <v>0.99863386886738936</v>
       </c>
     </row>
-    <row r="258" spans="1:9" ht="20.399999999999999">
+    <row r="258" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A258" s="8" t="s">
         <v>61</v>
       </c>
@@ -8270,7 +8276,7 @@
         <v>1.038377680713447</v>
       </c>
     </row>
-    <row r="259" spans="1:9" ht="20.399999999999999">
+    <row r="259" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A259" s="8" t="s">
         <v>62</v>
       </c>
@@ -8299,7 +8305,7 @@
         <v>0.84094833789034396</v>
       </c>
     </row>
-    <row r="260" spans="1:9" ht="20.399999999999999">
+    <row r="260" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A260" s="8" t="s">
         <v>62</v>
       </c>
@@ -8328,7 +8334,7 @@
         <v>0.91875923190546527</v>
       </c>
     </row>
-    <row r="261" spans="1:9" ht="20.399999999999999">
+    <row r="261" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A261" s="8" t="s">
         <v>62</v>
       </c>
@@ -8357,7 +8363,7 @@
         <v>0.91949671750630102</v>
       </c>
     </row>
-    <row r="262" spans="1:9" ht="20.399999999999999">
+    <row r="262" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A262" s="8" t="s">
         <v>62</v>
       </c>
@@ -8386,7 +8392,7 @@
         <v>0.88394062078272606</v>
       </c>
     </row>
-    <row r="263" spans="1:9" ht="20.399999999999999">
+    <row r="263" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A263" s="8" t="s">
         <v>62</v>
       </c>
@@ -8415,7 +8421,7 @@
         <v>0.94972236550656919</v>
       </c>
     </row>
-    <row r="264" spans="1:9" ht="20.399999999999999">
+    <row r="264" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A264" s="8" t="s">
         <v>62</v>
       </c>
@@ -8444,7 +8450,7 @@
         <v>0.85852076664033594</v>
       </c>
     </row>
-    <row r="265" spans="1:9" ht="20.399999999999999">
+    <row r="265" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A265" s="8" t="s">
         <v>62</v>
       </c>
@@ -8473,7 +8479,7 @@
         <v>0.6277314263011522</v>
       </c>
     </row>
-    <row r="266" spans="1:9" ht="20.399999999999999">
+    <row r="266" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A266" s="8" t="s">
         <v>62</v>
       </c>
@@ -8502,7 +8508,7 @@
         <v>1.0109676552372879</v>
       </c>
     </row>
-    <row r="267" spans="1:9" ht="20.399999999999999">
+    <row r="267" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A267" s="8" t="s">
         <v>63</v>
       </c>
@@ -8531,7 +8537,7 @@
         <v>1.6413368466813942</v>
       </c>
     </row>
-    <row r="268" spans="1:9" ht="20.399999999999999">
+    <row r="268" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A268" s="8" t="s">
         <v>63</v>
       </c>
@@ -8560,7 +8566,7 @@
         <v>1.1773541794486639</v>
       </c>
     </row>
-    <row r="269" spans="1:9" ht="20.399999999999999">
+    <row r="269" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A269" s="8" t="s">
         <v>63</v>
       </c>
@@ -8589,7 +8595,7 @@
         <v>0.93517350309637781</v>
       </c>
     </row>
-    <row r="270" spans="1:9" ht="20.399999999999999">
+    <row r="270" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A270" s="8" t="s">
         <v>63</v>
       </c>
@@ -8618,7 +8624,7 @@
         <v>0.74969770253929868</v>
       </c>
     </row>
-    <row r="271" spans="1:9" ht="20.399999999999999">
+    <row r="271" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A271" s="8" t="s">
         <v>63</v>
       </c>
@@ -8647,7 +8653,7 @@
         <v>0.6623259991019308</v>
       </c>
     </row>
-    <row r="272" spans="1:9" ht="20.399999999999999">
+    <row r="272" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A272" s="8" t="s">
         <v>63</v>
       </c>
@@ -8676,7 +8682,7 @@
         <v>1.1594824226362148</v>
       </c>
     </row>
-    <row r="273" spans="1:9" ht="20.399999999999999">
+    <row r="273" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A273" s="8" t="s">
         <v>64</v>
       </c>
@@ -8705,7 +8711,7 @@
         <v>3.1265907841420457</v>
       </c>
     </row>
-    <row r="274" spans="1:9" ht="20.399999999999999">
+    <row r="274" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A274" s="8" t="s">
         <v>64</v>
       </c>
@@ -8734,7 +8740,7 @@
         <v>2.5086161493897086</v>
       </c>
     </row>
-    <row r="275" spans="1:9" ht="20.399999999999999">
+    <row r="275" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A275" s="8" t="s">
         <v>64</v>
       </c>
@@ -8763,7 +8769,7 @@
         <v>3.0569282643212672</v>
       </c>
     </row>
-    <row r="276" spans="1:9" ht="20.399999999999999">
+    <row r="276" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A276" s="8" t="s">
         <v>64</v>
       </c>
@@ -8792,7 +8798,7 @@
         <v>2.3316382203372381</v>
       </c>
     </row>
-    <row r="277" spans="1:9" ht="20.399999999999999">
+    <row r="277" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A277" s="8" t="s">
         <v>64</v>
       </c>
@@ -8821,7 +8827,7 @@
         <v>2.6655500287618854</v>
       </c>
     </row>
-    <row r="278" spans="1:9" ht="20.399999999999999">
+    <row r="278" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A278" s="8" t="s">
         <v>64</v>
       </c>
@@ -8850,7 +8856,7 @@
         <v>2.4676656069753236</v>
       </c>
     </row>
-    <row r="279" spans="1:9" ht="20.399999999999999">
+    <row r="279" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A279" s="8" t="s">
         <v>64</v>
       </c>
@@ -8879,7 +8885,7 @@
         <v>1.748241311031731</v>
       </c>
     </row>
-    <row r="280" spans="1:9" ht="20.399999999999999">
+    <row r="280" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A280" s="8" t="s">
         <v>64</v>
       </c>
@@ -8908,7 +8914,7 @@
         <v>2.9450605112248773</v>
       </c>
     </row>
-    <row r="281" spans="1:9" ht="20.399999999999999">
+    <row r="281" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A281" s="8" t="s">
         <v>65</v>
       </c>
@@ -8937,7 +8943,7 @@
         <v>1.8912475876944035</v>
       </c>
     </row>
-    <row r="282" spans="1:9" ht="20.399999999999999">
+    <row r="282" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A282" s="8" t="s">
         <v>65</v>
       </c>
@@ -8966,7 +8972,7 @@
         <v>1.1731668656190681</v>
       </c>
     </row>
-    <row r="283" spans="1:9" ht="20.399999999999999">
+    <row r="283" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A283" s="8" t="s">
         <v>66</v>
       </c>
@@ -8995,7 +9001,7 @@
         <v>1.8232994526974198</v>
       </c>
     </row>
-    <row r="284" spans="1:9" ht="20.399999999999999">
+    <row r="284" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A284" s="8" t="s">
         <v>66</v>
       </c>
@@ -9024,7 +9030,7 @@
         <v>1.7889264790824326</v>
       </c>
     </row>
-    <row r="285" spans="1:9" ht="20.399999999999999">
+    <row r="285" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A285" s="8" t="s">
         <v>66</v>
       </c>
@@ -9053,7 +9059,7 @@
         <v>1.9181843492285979</v>
       </c>
     </row>
-    <row r="286" spans="1:9" ht="20.399999999999999">
+    <row r="286" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A286" s="8" t="s">
         <v>66</v>
       </c>
@@ -9082,7 +9088,7 @@
         <v>1.7726402770604854</v>
       </c>
     </row>
-    <row r="287" spans="1:9" ht="20.399999999999999">
+    <row r="287" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A287" s="9" t="s">
         <v>66</v>
       </c>
@@ -9111,7 +9117,7 @@
         <v>1.4933586623848507</v>
       </c>
     </row>
-    <row r="288" spans="1:9" ht="20.399999999999999">
+    <row r="288" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A288" s="9" t="s">
         <v>66</v>
       </c>
@@ -9140,7 +9146,7 @@
         <v>1.7934725272617416</v>
       </c>
     </row>
-    <row r="289" spans="1:9" ht="20.399999999999999">
+    <row r="289" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A289" s="9" t="s">
         <v>66</v>
       </c>
@@ -9169,7 +9175,7 @@
         <v>1.7706949977866313</v>
       </c>
     </row>
-    <row r="290" spans="1:9" ht="20.399999999999999">
+    <row r="290" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A290" s="7" t="s">
         <v>67</v>
       </c>
@@ -9198,7 +9204,7 @@
         <v>2.0571600180189198</v>
       </c>
     </row>
-    <row r="291" spans="1:9" ht="20.399999999999999">
+    <row r="291" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A291" s="9" t="s">
         <v>68</v>
       </c>
@@ -9227,7 +9233,7 @@
         <v>1.9957475155817965</v>
       </c>
     </row>
-    <row r="292" spans="1:9" ht="20.399999999999999">
+    <row r="292" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A292" s="9" t="s">
         <v>68</v>
       </c>
@@ -9256,7 +9262,7 @@
         <v>2.2846692019624348</v>
       </c>
     </row>
-    <row r="293" spans="1:9" ht="20.399999999999999">
+    <row r="293" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A293" s="9" t="s">
         <v>68</v>
       </c>
@@ -9285,7 +9291,7 @@
         <v>2.1153377774971358</v>
       </c>
     </row>
-    <row r="294" spans="1:9" ht="20.399999999999999">
+    <row r="294" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A294" s="8" t="s">
         <v>69</v>
       </c>
@@ -9314,7 +9320,7 @@
         <v>0.97296199540289308</v>
       </c>
     </row>
-    <row r="295" spans="1:9" ht="20.399999999999999">
+    <row r="295" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A295" s="8" t="s">
         <v>69</v>
       </c>
@@ -9343,7 +9349,7 @@
         <v>1.0492511548513399</v>
       </c>
     </row>
-    <row r="296" spans="1:9" ht="20.399999999999999">
+    <row r="296" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A296" s="8" t="s">
         <v>69</v>
       </c>
@@ -9372,7 +9378,7 @@
         <v>1.4385835485060863</v>
       </c>
     </row>
-    <row r="297" spans="1:9" ht="20.399999999999999">
+    <row r="297" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A297" s="8" t="s">
         <v>70</v>
       </c>
@@ -9401,7 +9407,7 @@
         <v>2.4419877900610496</v>
       </c>
     </row>
-    <row r="298" spans="1:9" ht="20.399999999999999">
+    <row r="298" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A298" s="8" t="s">
         <v>70</v>
       </c>
@@ -9430,7 +9436,7 @@
         <v>1.6876910169593096</v>
       </c>
     </row>
-    <row r="299" spans="1:9" ht="20.399999999999999">
+    <row r="299" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A299" s="8" t="s">
         <v>70</v>
       </c>
@@ -9459,7 +9465,7 @@
         <v>1.8381463035361945</v>
       </c>
     </row>
-    <row r="300" spans="1:9" ht="20.399999999999999">
+    <row r="300" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A300" s="7" t="s">
         <v>71</v>
       </c>
@@ -9488,7 +9494,7 @@
         <v>1.7357214466340471</v>
       </c>
     </row>
-    <row r="301" spans="1:9" ht="20.399999999999999">
+    <row r="301" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A301" s="9" t="s">
         <v>72</v>
       </c>
@@ -9517,7 +9523,7 @@
         <v>1.6991079683166337</v>
       </c>
     </row>
-    <row r="302" spans="1:9" ht="20.399999999999999">
+    <row r="302" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A302" s="9" t="s">
         <v>72</v>
       </c>
@@ -9546,7 +9552,7 @@
         <v>1.1427555871506643</v>
       </c>
     </row>
-    <row r="303" spans="1:9" ht="20.399999999999999">
+    <row r="303" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A303" s="9" t="s">
         <v>72</v>
       </c>
@@ -9575,7 +9581,7 @@
         <v>1.1629497879326858</v>
       </c>
     </row>
-    <row r="304" spans="1:9" ht="20.399999999999999">
+    <row r="304" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A304" s="8" t="s">
         <v>73</v>
       </c>
@@ -9604,7 +9610,7 @@
         <v>1.5848917719044004</v>
       </c>
     </row>
-    <row r="305" spans="1:9" ht="20.399999999999999">
+    <row r="305" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A305" s="8" t="s">
         <v>73</v>
       </c>
@@ -9633,7 +9639,7 @@
         <v>1.0340301565451229</v>
       </c>
     </row>
-    <row r="306" spans="1:9" ht="20.399999999999999">
+    <row r="306" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A306" s="8" t="s">
         <v>73</v>
       </c>
@@ -9662,7 +9668,7 @@
         <v>0.8424887573290829</v>
       </c>
     </row>
-    <row r="307" spans="1:9" ht="20.399999999999999">
+    <row r="307" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A307" s="8" t="s">
         <v>73</v>
       </c>
@@ -9691,7 +9697,7 @@
         <v>0.86316860351371449</v>
       </c>
     </row>
-    <row r="308" spans="1:9" ht="20.399999999999999">
+    <row r="308" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A308" s="8" t="s">
         <v>74</v>
       </c>
@@ -9720,7 +9726,7 @@
         <v>2.7683581607524927</v>
       </c>
     </row>
-    <row r="309" spans="1:9" ht="20.399999999999999">
+    <row r="309" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A309" s="8" t="s">
         <v>74</v>
       </c>
@@ -9749,7 +9755,7 @@
         <v>1.7497139890594806</v>
       </c>
     </row>
-    <row r="310" spans="1:9" ht="20.399999999999999">
+    <row r="310" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A310" s="8" t="s">
         <v>74</v>
       </c>
@@ -9778,7 +9784,7 @@
         <v>2.4048057358783064</v>
       </c>
     </row>
-    <row r="311" spans="1:9" ht="20.399999999999999">
+    <row r="311" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A311" s="8" t="s">
         <v>74</v>
       </c>
@@ -9807,7 +9813,7 @@
         <v>1.7883599893629145</v>
       </c>
     </row>
-    <row r="312" spans="1:9" ht="20.399999999999999">
+    <row r="312" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A312" s="8" t="s">
         <v>74</v>
       </c>
@@ -9836,7 +9842,7 @@
         <v>1.5974886641088246</v>
       </c>
     </row>
-    <row r="313" spans="1:9" ht="20.399999999999999">
+    <row r="313" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A313" s="8" t="s">
         <v>74</v>
       </c>
@@ -9865,7 +9871,7 @@
         <v>1.5481508464502771</v>
       </c>
     </row>
-    <row r="314" spans="1:9" ht="20.399999999999999">
+    <row r="314" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A314" s="8" t="s">
         <v>75</v>
       </c>
@@ -9894,7 +9900,7 @@
         <v>1.3022407927153932</v>
       </c>
     </row>
-    <row r="315" spans="1:9" ht="20.399999999999999">
+    <row r="315" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A315" s="8" t="s">
         <v>75</v>
       </c>
@@ -9923,7 +9929,7 @@
         <v>1.41865776528461</v>
       </c>
     </row>
-    <row r="316" spans="1:9" ht="20.399999999999999">
+    <row r="316" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A316" s="8" t="s">
         <v>75</v>
       </c>
@@ -9952,7 +9958,7 @@
         <v>0.69526812663330151</v>
       </c>
     </row>
-    <row r="317" spans="1:9" ht="20.399999999999999">
+    <row r="317" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A317" s="8" t="s">
         <v>75</v>
       </c>
@@ -9981,7 +9987,7 @@
         <v>0.80605764533463609</v>
       </c>
     </row>
-    <row r="318" spans="1:9" ht="20.399999999999999">
+    <row r="318" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A318" s="8" t="s">
         <v>75</v>
       </c>
@@ -10010,7 +10016,7 @@
         <v>0.86149124425753443</v>
       </c>
     </row>
-    <row r="319" spans="1:9" ht="20.399999999999999">
+    <row r="319" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A319" s="8" t="s">
         <v>75</v>
       </c>
@@ -10039,7 +10045,7 @@
         <v>0.71799632607106878</v>
       </c>
     </row>
-    <row r="320" spans="1:9" ht="20.399999999999999">
+    <row r="320" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A320" s="8" t="s">
         <v>75</v>
       </c>
@@ -10068,7 +10074,7 @@
         <v>0.91125078944994131</v>
       </c>
     </row>
-    <row r="321" spans="1:9" ht="20.399999999999999">
+    <row r="321" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A321" s="8" t="s">
         <v>76</v>
       </c>
@@ -10097,7 +10103,7 @@
         <v>1.4407348376814026</v>
       </c>
     </row>
-    <row r="322" spans="1:9" ht="20.399999999999999">
+    <row r="322" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A322" s="8" t="s">
         <v>76</v>
       </c>
@@ -10126,7 +10132,7 @@
         <v>0.73627607398215444</v>
       </c>
     </row>
-    <row r="323" spans="1:9" ht="20.399999999999999">
+    <row r="323" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A323" s="7" t="s">
         <v>76</v>
       </c>
@@ -10155,7 +10161,7 @@
         <v>1.0698023960037133</v>
       </c>
     </row>
-    <row r="324" spans="1:9" ht="20.399999999999999">
+    <row r="324" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A324" s="8" t="s">
         <v>77</v>
       </c>
@@ -10184,7 +10190,7 @@
         <v>1.0529786532509386</v>
       </c>
     </row>
-    <row r="325" spans="1:9" ht="20.399999999999999">
+    <row r="325" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A325" s="8" t="s">
         <v>77</v>
       </c>
@@ -10213,7 +10219,7 @@
         <v>0.74804832504668273</v>
       </c>
     </row>
-    <row r="326" spans="1:9" ht="20.399999999999999">
+    <row r="326" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A326" s="8" t="s">
         <v>77</v>
       </c>
@@ -10242,7 +10248,7 @@
         <v>0.61547786960728312</v>
       </c>
     </row>
-    <row r="327" spans="1:9" ht="20.399999999999999">
+    <row r="327" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A327" s="7" t="s">
         <v>78</v>
       </c>
@@ -10271,7 +10277,7 @@
         <v>1.711195600438121</v>
       </c>
     </row>
-    <row r="328" spans="1:9" ht="20.399999999999999">
+    <row r="328" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A328" s="11" t="s">
         <v>79</v>
       </c>
@@ -10300,7 +10306,7 @@
         <v>1.1361569753529552</v>
       </c>
     </row>
-    <row r="329" spans="1:9" ht="20.399999999999999">
+    <row r="329" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A329" s="11" t="s">
         <v>79</v>
       </c>
@@ -10329,7 +10335,7 @@
         <v>0.85659147595900009</v>
       </c>
     </row>
-    <row r="330" spans="1:9" ht="20.399999999999999">
+    <row r="330" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A330" s="8" t="s">
         <v>80</v>
       </c>
@@ -10358,7 +10364,7 @@
         <v>2.0601271921372133</v>
       </c>
     </row>
-    <row r="331" spans="1:9" ht="20.399999999999999">
+    <row r="331" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A331" s="8" t="s">
         <v>80</v>
       </c>
@@ -10387,7 +10393,7 @@
         <v>1.0322855897383578</v>
       </c>
     </row>
-    <row r="332" spans="1:9" ht="20.399999999999999">
+    <row r="332" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A332" s="8" t="s">
         <v>80</v>
       </c>
@@ -10416,7 +10422,7 @@
         <v>0.7918469856886371</v>
       </c>
     </row>
-    <row r="333" spans="1:9" ht="20.399999999999999">
+    <row r="333" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A333" s="8" t="s">
         <v>80</v>
       </c>
@@ -10445,7 +10451,7 @@
         <v>0.85579803166452717</v>
       </c>
     </row>
-    <row r="334" spans="1:9" ht="20.399999999999999">
+    <row r="334" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A334" s="8" t="s">
         <v>80</v>
       </c>
@@ -10474,7 +10480,7 @@
         <v>0.69103419884141504</v>
       </c>
     </row>
-    <row r="335" spans="1:9" ht="20.399999999999999">
+    <row r="335" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A335" s="8" t="s">
         <v>80</v>
       </c>
@@ -10503,7 +10509,7 @@
         <v>1.0446926366310016</v>
       </c>
     </row>
-    <row r="336" spans="1:9" ht="20.399999999999999">
+    <row r="336" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A336" s="8" t="s">
         <v>80</v>
       </c>
@@ -10532,7 +10538,7 @@
         <v>0.90268898261417208</v>
       </c>
     </row>
-    <row r="337" spans="1:9" ht="20.399999999999999">
+    <row r="337" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A337" s="8" t="s">
         <v>80</v>
       </c>
@@ -10561,7 +10567,7 @@
         <v>0.72707791213837436</v>
       </c>
     </row>
-    <row r="338" spans="1:9" ht="20.399999999999999">
+    <row r="338" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A338" s="8" t="s">
         <v>81</v>
       </c>
@@ -10590,7 +10596,7 @@
         <v>1.9801176160087703</v>
       </c>
     </row>
-    <row r="339" spans="1:9" ht="20.399999999999999">
+    <row r="339" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A339" s="8" t="s">
         <v>81</v>
       </c>
@@ -10619,7 +10625,7 @@
         <v>1.257992827515384</v>
       </c>
     </row>
-    <row r="340" spans="1:9" ht="20.399999999999999">
+    <row r="340" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A340" s="8" t="s">
         <v>82</v>
       </c>
@@ -10648,7 +10654,7 @@
         <v>1.2459663874100391</v>
       </c>
     </row>
-    <row r="341" spans="1:9" ht="20.399999999999999">
+    <row r="341" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A341" s="8" t="s">
         <v>82</v>
       </c>
@@ -10677,7 +10683,7 @@
         <v>1.690055039704214</v>
       </c>
     </row>
-    <row r="342" spans="1:9" ht="20.399999999999999">
+    <row r="342" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A342" s="8" t="s">
         <v>83</v>
       </c>
@@ -10706,7 +10712,7 @@
         <v>2.0568425028326827</v>
       </c>
     </row>
-    <row r="343" spans="1:9" ht="20.399999999999999">
+    <row r="343" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A343" s="8" t="s">
         <v>83</v>
       </c>
@@ -10735,7 +10741,7 @@
         <v>0.91882077064153211</v>
       </c>
     </row>
-    <row r="344" spans="1:9" ht="20.399999999999999">
+    <row r="344" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A344" s="8" t="s">
         <v>83</v>
       </c>
@@ -10764,7 +10770,7 @@
         <v>1.589348976508733</v>
       </c>
     </row>
-    <row r="345" spans="1:9" ht="20.399999999999999">
+    <row r="345" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A345" s="8" t="s">
         <v>83</v>
       </c>
@@ -10793,7 +10799,7 @@
         <v>0.71834681828121583</v>
       </c>
     </row>
-    <row r="346" spans="1:9" ht="20.399999999999999">
+    <row r="346" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A346" s="8" t="s">
         <v>83</v>
       </c>
@@ -10822,7 +10828,7 @@
         <v>0.81786461967899515</v>
       </c>
     </row>
-    <row r="347" spans="1:9" ht="20.399999999999999">
+    <row r="347" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A347" s="8" t="s">
         <v>83</v>
       </c>
@@ -10851,7 +10857,7 @@
         <v>0.98993744900734293</v>
       </c>
     </row>
-    <row r="348" spans="1:9" ht="20.399999999999999">
+    <row r="348" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A348" s="8" t="s">
         <v>83</v>
       </c>
@@ -10880,7 +10886,7 @@
         <v>0.84329992419775968</v>
       </c>
     </row>
-    <row r="349" spans="1:9" ht="20.399999999999999">
+    <row r="349" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A349" s="8" t="s">
         <v>83</v>
       </c>
@@ -10909,7 +10915,7 @@
         <v>0.82947838570744936</v>
       </c>
     </row>
-    <row r="350" spans="1:9" ht="20.399999999999999">
+    <row r="350" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A350" s="8" t="s">
         <v>83</v>
       </c>
@@ -10938,7 +10944,7 @@
         <v>0.85359517321089629</v>
       </c>
     </row>
-    <row r="351" spans="1:9" ht="20.399999999999999">
+    <row r="351" spans="1:9" ht="20.399999999999999" hidden="1">
       <c r="A351" s="8" t="s">
         <v>83</v>
       </c>
@@ -10968,6 +10974,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I351">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="เชียงใหม่"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>